<commit_message>
Added Convenience Features to GPCASM
Basic Assembling of Programs working,
Assembling of multiple files
Adding Strings In File
Adding Relative Memory Resolver to Labels
</commit_message>
<xml_diff>
--- a/Documantation/Instruction Table.xlsx
+++ b/Documantation/Instruction Table.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\GPC Emulator\Documantation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2326B0-383D-4019-8865-A87C77BDB4BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0E4F9F-61C8-45AD-9A69-37366ACFDFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3870" windowWidth="19440" windowHeight="11640" xr2:uid="{3C5A492D-A658-4387-B086-5FF5A886E6D7}"/>
+    <workbookView xWindow="28680" yWindow="3930" windowWidth="19440" windowHeight="11640" xr2:uid="{3C5A492D-A658-4387-B086-5FF5A886E6D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -606,7 +605,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>